<commit_message>
WMSE and Detailed diff report functionality ready
</commit_message>
<xml_diff>
--- a/output/ssp/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
+++ b/output/ssp/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
@@ -838,112 +838,112 @@
         <v>0.5</v>
       </c>
       <c r="J4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="K4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="L4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="M4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="N4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="O4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="P4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="Q4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="R4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="S4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="T4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="U4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="V4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="W4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="X4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="Y4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="Z4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AA4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AB4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AC4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AD4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AE4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AF4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AG4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AH4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AI4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AJ4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AK4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AL4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AM4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AN4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AO4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AP4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AQ4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AR4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
       <c r="AS4">
-        <v>0.3142625113544965</v>
+        <v>1.016025614293143</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -960,112 +960,112 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="K5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="L5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="M5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="N5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="O5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="P5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="Q5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="R5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="S5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="T5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="U5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="V5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="W5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="X5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="Y5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="Z5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AA5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AB5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AC5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AD5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AE5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AF5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AG5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AH5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AI5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AJ5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AK5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AL5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AM5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AN5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AO5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AP5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AQ5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AR5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
       <c r="AS5">
-        <v>-0.07815492933251093</v>
+        <v>-0.1315854458144212</v>
       </c>
     </row>
     <row r="6" spans="1:45">

</xml_diff>

<commit_message>
Add optimization log flag and conditional loading of scale values
</commit_message>
<xml_diff>
--- a/output/ssp/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
+++ b/output/ssp/templates/calibrated/croatia/model_input_variables_croatia_se_calibrated.xlsx
@@ -838,112 +838,112 @@
         <v>0.5</v>
       </c>
       <c r="J4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="K4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="L4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="M4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="N4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="O4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="P4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="Q4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="R4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="S4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="T4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="U4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="V4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="W4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="X4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="Y4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="Z4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AA4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AB4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AC4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AD4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AE4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AF4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AG4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AH4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AI4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AJ4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AK4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AL4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AM4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AN4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AO4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AP4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AQ4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AR4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
       <c r="AS4">
-        <v>1.016025614293143</v>
+        <v>0.6193541768728235</v>
       </c>
     </row>
     <row r="5" spans="1:45">
@@ -960,112 +960,112 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="K5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="L5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="M5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="N5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="O5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="P5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="Q5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="R5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="S5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="T5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="U5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="V5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="W5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="X5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="Y5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="Z5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AA5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AB5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AC5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AD5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AE5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AF5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AG5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AH5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AI5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AJ5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AK5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AL5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AM5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AN5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AO5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AP5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AQ5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AR5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
       <c r="AS5">
-        <v>-0.1315854458144212</v>
+        <v>-0.07866934995703223</v>
       </c>
     </row>
     <row r="6" spans="1:45">

</xml_diff>